<commit_message>
added a new code for Arduino, because they will have different codes
ok
</commit_message>
<xml_diff>
--- a/Pin assignments.xlsx
+++ b/Pin assignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Signal</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Remove</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Change</t>
@@ -117,7 +114,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +126,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -205,6 +208,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -490,7 +496,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,17 +623,17 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="9">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -641,7 +647,7 @@
         <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -743,8 +749,8 @@
       <c r="B22" s="4">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>26</v>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
apparently i changed pin assignments again
lol
</commit_message>
<xml_diff>
--- a/Pin assignments.xlsx
+++ b/Pin assignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Signal</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
added bat check, left, and right pinouts
yeah
</commit_message>
<xml_diff>
--- a/Pin assignments.xlsx
+++ b/Pin assignments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Signal</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>MISO</t>
   </si>
   <si>
@@ -111,6 +105,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Bat. Check</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Left Button</t>
+  </si>
+  <si>
+    <t>Right Button</t>
   </si>
 </sst>
 </file>
@@ -499,9 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="204" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="256" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -515,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -566,11 +574,11 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
+      <c r="D4" s="2">
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -583,11 +591,11 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
+      <c r="D5" s="2">
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,7 +628,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -643,125 +651,149 @@
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2">
-        <v>3</v>
-      </c>
-      <c r="D17" s="7">
-        <v>23</v>
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="7">
-        <v>18</v>
-      </c>
-      <c r="E18" s="8">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="5">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="D19" s="7">
+        <v>18</v>
       </c>
       <c r="E19" s="8">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E20" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5">
+        <v>19</v>
+      </c>
+      <c r="E21" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="2">
         <v>7</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D22" s="5">
         <v>21</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E22" s="8">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B23" s="4">
         <v>8</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="8" t="s">
-        <v>26</v>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>